<commit_message>
compilations are now fully working with the current database
</commit_message>
<xml_diff>
--- a/vgp_database/Beaver_River_intrusions.xlsx
+++ b/vgp_database/Beaver_River_intrusions.xlsx
@@ -730,8 +730,9 @@
     <col customWidth="1" min="25" max="25" width="16.86"/>
     <col customWidth="1" min="26" max="26" width="11.14"/>
     <col customWidth="1" min="27" max="31" width="10.71"/>
-    <col customWidth="1" min="32" max="32" width="15.29"/>
-    <col customWidth="1" min="33" max="43" width="10.71"/>
+    <col customWidth="1" min="32" max="32" width="13.71"/>
+    <col customWidth="1" min="33" max="33" width="14.0"/>
+    <col customWidth="1" min="34" max="43" width="10.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1383,9 +1384,11 @@
       <c r="AC9" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="AD9" s="12"/>
+      <c r="AD9" s="32"/>
       <c r="AE9" s="32"/>
-      <c r="AF9" s="12"/>
+      <c r="AF9" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG9" s="20">
         <v>1.0</v>
       </c>
@@ -1479,7 +1482,9 @@
       </c>
       <c r="AD10" s="12"/>
       <c r="AE10" s="12"/>
-      <c r="AF10" s="12"/>
+      <c r="AF10" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG10" s="20">
         <v>1.0</v>
       </c>
@@ -1573,7 +1578,9 @@
       </c>
       <c r="AD11" s="12"/>
       <c r="AE11" s="12"/>
-      <c r="AF11" s="12"/>
+      <c r="AF11" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG11" s="20">
         <v>1.0</v>
       </c>
@@ -1667,7 +1674,9 @@
       </c>
       <c r="AD12" s="12"/>
       <c r="AE12" s="12"/>
-      <c r="AF12" s="12"/>
+      <c r="AF12" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG12" s="20">
         <v>1.0</v>
       </c>
@@ -1761,7 +1770,9 @@
       </c>
       <c r="AD13" s="12"/>
       <c r="AE13" s="12"/>
-      <c r="AF13" s="12"/>
+      <c r="AF13" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG13" s="20">
         <v>1.0</v>
       </c>
@@ -1855,7 +1866,9 @@
       </c>
       <c r="AD14" s="12"/>
       <c r="AE14" s="12"/>
-      <c r="AF14" s="12"/>
+      <c r="AF14" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG14" s="20">
         <v>1.0</v>
       </c>
@@ -1949,7 +1962,9 @@
       </c>
       <c r="AD15" s="12"/>
       <c r="AE15" s="12"/>
-      <c r="AF15" s="12"/>
+      <c r="AF15" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG15" s="20">
         <v>1.0</v>
       </c>
@@ -2043,7 +2058,9 @@
       </c>
       <c r="AD16" s="12"/>
       <c r="AE16" s="12"/>
-      <c r="AF16" s="12"/>
+      <c r="AF16" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG16" s="20">
         <v>1.0</v>
       </c>
@@ -2137,7 +2154,9 @@
       </c>
       <c r="AD17" s="12"/>
       <c r="AE17" s="12"/>
-      <c r="AF17" s="12"/>
+      <c r="AF17" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG17" s="20">
         <v>0.0</v>
       </c>
@@ -2233,7 +2252,9 @@
       </c>
       <c r="AD18" s="12"/>
       <c r="AE18" s="12"/>
-      <c r="AF18" s="12"/>
+      <c r="AF18" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG18" s="20">
         <v>1.0</v>
       </c>
@@ -2327,7 +2348,9 @@
       </c>
       <c r="AD19" s="12"/>
       <c r="AE19" s="12"/>
-      <c r="AF19" s="12"/>
+      <c r="AF19" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG19" s="20">
         <v>1.0</v>
       </c>
@@ -2421,7 +2444,9 @@
       </c>
       <c r="AD20" s="12"/>
       <c r="AE20" s="12"/>
-      <c r="AF20" s="12"/>
+      <c r="AF20" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG20" s="20">
         <v>1.0</v>
       </c>
@@ -2515,7 +2540,9 @@
       </c>
       <c r="AD21" s="12"/>
       <c r="AE21" s="12"/>
-      <c r="AF21" s="12"/>
+      <c r="AF21" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG21" s="20">
         <v>0.0</v>
       </c>
@@ -2611,7 +2638,9 @@
       </c>
       <c r="AD22" s="12"/>
       <c r="AE22" s="12"/>
-      <c r="AF22" s="12"/>
+      <c r="AF22" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG22" s="20">
         <v>1.0</v>
       </c>
@@ -2705,7 +2734,9 @@
       </c>
       <c r="AD23" s="12"/>
       <c r="AE23" s="12"/>
-      <c r="AF23" s="12"/>
+      <c r="AF23" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG23" s="20">
         <v>1.0</v>
       </c>
@@ -2799,7 +2830,9 @@
       </c>
       <c r="AD24" s="12"/>
       <c r="AE24" s="12"/>
-      <c r="AF24" s="12"/>
+      <c r="AF24" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG24" s="20">
         <v>0.0</v>
       </c>
@@ -2895,7 +2928,9 @@
       </c>
       <c r="AD25" s="12"/>
       <c r="AE25" s="12"/>
-      <c r="AF25" s="12"/>
+      <c r="AF25" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG25" s="20">
         <v>1.0</v>
       </c>
@@ -2989,7 +3024,9 @@
       </c>
       <c r="AD26" s="12"/>
       <c r="AE26" s="12"/>
-      <c r="AF26" s="12"/>
+      <c r="AF26" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG26" s="20">
         <v>1.0</v>
       </c>
@@ -3083,7 +3120,9 @@
       </c>
       <c r="AD27" s="12"/>
       <c r="AE27" s="12"/>
-      <c r="AF27" s="12"/>
+      <c r="AF27" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG27" s="20">
         <v>1.0</v>
       </c>
@@ -3177,7 +3216,9 @@
       </c>
       <c r="AD28" s="12"/>
       <c r="AE28" s="12"/>
-      <c r="AF28" s="12"/>
+      <c r="AF28" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG28" s="20">
         <v>1.0</v>
       </c>
@@ -3271,7 +3312,9 @@
       </c>
       <c r="AD29" s="12"/>
       <c r="AE29" s="12"/>
-      <c r="AF29" s="12"/>
+      <c r="AF29" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG29" s="20">
         <v>1.0</v>
       </c>
@@ -3365,7 +3408,9 @@
       </c>
       <c r="AD30" s="12"/>
       <c r="AE30" s="12"/>
-      <c r="AF30" s="12"/>
+      <c r="AF30" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG30" s="20">
         <v>1.0</v>
       </c>
@@ -3459,7 +3504,9 @@
       </c>
       <c r="AD31" s="12"/>
       <c r="AE31" s="12"/>
-      <c r="AF31" s="12"/>
+      <c r="AF31" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG31" s="20">
         <v>1.0</v>
       </c>
@@ -3553,7 +3600,9 @@
       </c>
       <c r="AD32" s="12"/>
       <c r="AE32" s="12"/>
-      <c r="AF32" s="12"/>
+      <c r="AF32" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG32" s="20">
         <v>0.0</v>
       </c>
@@ -3649,7 +3698,9 @@
       </c>
       <c r="AD33" s="12"/>
       <c r="AE33" s="12"/>
-      <c r="AF33" s="12"/>
+      <c r="AF33" s="31">
+        <v>0.0</v>
+      </c>
       <c r="AG33" s="20">
         <v>1.0</v>
       </c>

</xml_diff>